<commit_message>
feat: add more entries to accepted papers
</commit_message>
<xml_diff>
--- a/data/accepted.xlsx
+++ b/data/accepted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\icmc-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2285A11-44DC-4766-A3F2-C03D95F0EFCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2689B3C-7F85-4DD2-AA7F-6C746538B246}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="4215" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="254">
   <si>
     <t>ID</t>
   </si>
@@ -260,13 +260,6 @@
   </si>
   <si>
     <t>Sl no</t>
-  </si>
-  <si>
-    <t>ICMC 2021
-LIST OF ACCEPTED PAPERS*</t>
-  </si>
-  <si>
-    <t>* Some more papers will be accepted based on reviewers' comments</t>
   </si>
   <si>
     <t>Konark Yadav
@@ -987,12 +980,101 @@
     <t>Ho Chi Minh City Open University, Vietnam
 Ho Chi Minh City Open University, Vietnam</t>
   </si>
+  <si>
+    <t>Real-time error correction codes for deletable errors</t>
+  </si>
+  <si>
+    <t>Ghurumuruhan Ganesan</t>
+  </si>
+  <si>
+    <t>Institute of Mathematical Sciences Chennai, India</t>
+  </si>
+  <si>
+    <t>Some Study on Solitary Traveling Wave Solutions for Nonlinear Evolution Equations</t>
+  </si>
+  <si>
+    <t>Jasvinderpal Singh Virdi</t>
+  </si>
+  <si>
+    <t>A study on randomness used in signature generation of UOV</t>
+  </si>
+  <si>
+    <t>Yasuhiko Ikematsu</t>
+  </si>
+  <si>
+    <t>Kyushu University, Japan</t>
+  </si>
+  <si>
+    <t>Prachi Gupta
+P R Mishra
+Atul Gaur</t>
+  </si>
+  <si>
+    <t>University of Delhi, India
+Defence Research and Development Organization, India
+Defence Research and Development Organization, India</t>
+  </si>
+  <si>
+    <t>Computing Prices for Target Profits in Contracts</t>
+  </si>
+  <si>
+    <t>On the solution of Bush and Wilson's stochastic model for two-choice behavior of the paradise fish approached by the fixed point method</t>
+  </si>
+  <si>
+    <t>Ali Turab
+Wutiphol Sintunavarat</t>
+  </si>
+  <si>
+    <t>Thammasat University, Thailand
+Thammasat University, Thailand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anupam Biswas
+Angshuman Bora
+Debashish Malakar
+Subham Chakraborty
+Suman Bera   </t>
+  </si>
+  <si>
+    <t>National Institute of Technology Silchar, India
+National Institute of Technology Silchar, India
+National Institute of Technology Silchar, India
+National Institute of Technology Silchar, India
+National Institute of Technology Silchar, India</t>
+  </si>
+  <si>
+    <t>Genetic Algorithm based Deep Learning Models: A Design Perspective</t>
+  </si>
+  <si>
+    <t>Debojyoti Sarkar
+Anupam Biswas
+Nilima Mishra</t>
+  </si>
+  <si>
+    <r>
+      <t>On differential uniformity &amp; nonlinearity of permutations on ℤ</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Source Sans Pro"/>
+        <family val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+  </si>
+  <si>
+    <t>ICMC 2021
+LIST OF ACCEPTED PAPERS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1027,6 +1109,13 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Alegreya Sans SC"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Source Sans Pro"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1319,10 +1408,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1337,7 +1426,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>80</v>
+        <v>253</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -1372,10 +1461,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -1389,10 +1478,10 @@
         <v>5</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1406,10 +1495,10 @@
         <v>6</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -1423,10 +1512,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1440,10 +1529,10 @@
         <v>8</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1457,10 +1546,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1474,10 +1563,10 @@
         <v>10</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -1491,78 +1580,78 @@
         <v>11</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="6">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>98</v>
+        <v>234</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>235</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>10</v>
       </c>
       <c r="B12" s="6">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>100</v>
+        <v>221</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="6">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="54" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>12</v>
       </c>
       <c r="B14" s="6">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -1570,67 +1659,67 @@
         <v>13</v>
       </c>
       <c r="B15" s="6">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>14</v>
       </c>
       <c r="B16" s="6">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>224</v>
+        <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>225</v>
+        <v>105</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="54" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>15</v>
       </c>
       <c r="B17" s="6">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>222</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>15</v>
+        <v>223</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>16</v>
       </c>
       <c r="B18" s="6">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>109</v>
+        <v>15</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1638,67 +1727,67 @@
         <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>18</v>
+        <v>107</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>18</v>
       </c>
       <c r="B20" s="6">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="81" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A21" s="8">
         <v>19</v>
       </c>
       <c r="B21" s="6">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>112</v>
+        <v>20</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="81" x14ac:dyDescent="0.2">
       <c r="A22" s="8">
         <v>20</v>
       </c>
       <c r="B22" s="6">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>227</v>
+        <v>23</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1706,84 +1795,84 @@
         <v>21</v>
       </c>
       <c r="B23" s="6">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>24</v>
+        <v>225</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A24" s="8">
         <v>22</v>
       </c>
       <c r="B24" s="6">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
+        <v>237</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>118</v>
+        <v>238</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>23</v>
       </c>
       <c r="B25" s="6">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>121</v>
+        <v>24</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>114</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>24</v>
       </c>
       <c r="B26" s="6">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>122</v>
+        <v>25</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="54" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>25</v>
       </c>
       <c r="B27" s="6">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>125</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1791,16 +1880,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="6">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>126</v>
+        <v>26</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -1808,67 +1897,67 @@
         <v>27</v>
       </c>
       <c r="B29" s="6">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>128</v>
+        <v>27</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A30" s="8">
         <v>28</v>
       </c>
       <c r="B30" s="6">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A31" s="8">
         <v>29</v>
       </c>
       <c r="B31" s="6">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A32" s="8">
         <v>30</v>
       </c>
       <c r="B32" s="6">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>134</v>
+        <v>29</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1876,16 +1965,16 @@
         <v>31</v>
       </c>
       <c r="B33" s="6">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1893,16 +1982,16 @@
         <v>32</v>
       </c>
       <c r="B34" s="6">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1910,33 +1999,33 @@
         <v>33</v>
       </c>
       <c r="B35" s="6">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>138</v>
+        <v>34</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A36" s="8">
         <v>34</v>
       </c>
       <c r="B36" s="6">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>140</v>
+        <v>18</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1944,50 +2033,50 @@
         <v>35</v>
       </c>
       <c r="B37" s="6">
+        <v>127</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:5" ht="54" x14ac:dyDescent="0.2">
       <c r="A38" s="8">
         <v>36</v>
       </c>
       <c r="B38" s="6">
+        <v>131</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>143</v>
-      </c>
       <c r="E38" s="5" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A39" s="8">
         <v>37</v>
       </c>
       <c r="B39" s="6">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -1995,33 +2084,33 @@
         <v>38</v>
       </c>
       <c r="B40" s="6">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A41" s="8">
         <v>39</v>
       </c>
       <c r="B41" s="6">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2029,67 +2118,67 @@
         <v>40</v>
       </c>
       <c r="B42" s="6">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="81" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A43" s="8">
         <v>41</v>
       </c>
       <c r="B43" s="6">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A44" s="8">
         <v>42</v>
       </c>
       <c r="B44" s="6">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="81" x14ac:dyDescent="0.2">
       <c r="A45" s="8">
         <v>43</v>
       </c>
       <c r="B45" s="6">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>230</v>
+        <v>44</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>150</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>155</v>
+        <v>227</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2097,152 +2186,152 @@
         <v>44</v>
       </c>
       <c r="B46" s="6">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>157</v>
+        <v>45</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>151</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A47" s="8">
         <v>45</v>
       </c>
       <c r="B47" s="6">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>47</v>
+        <v>239</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>159</v>
+        <v>240</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A48" s="8">
         <v>46</v>
       </c>
       <c r="B48" s="6">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>48</v>
+        <v>252</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>161</v>
+        <v>242</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A49" s="8">
         <v>47</v>
       </c>
       <c r="B49" s="6">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D49" s="6" t="s">
-        <v>164</v>
+        <v>46</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>228</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A50" s="8">
         <v>48</v>
       </c>
       <c r="B50" s="6">
-        <v>195</v>
+        <v>164</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>166</v>
+        <v>154</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A51" s="8">
         <v>49</v>
       </c>
-      <c r="B51" s="8">
-        <v>204</v>
+      <c r="B51" s="6">
+        <v>166</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="54" x14ac:dyDescent="0.2">
       <c r="A52" s="8">
         <v>50</v>
       </c>
-      <c r="B52" s="8">
-        <v>205</v>
+      <c r="B52" s="6">
+        <v>167</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A53" s="8">
         <v>51</v>
       </c>
-      <c r="B53" s="8">
-        <v>206</v>
+      <c r="B53" s="6">
+        <v>191</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>170</v>
+        <v>161</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="54" x14ac:dyDescent="0.2">
       <c r="A54" s="8">
         <v>52</v>
       </c>
-      <c r="B54" s="8">
-        <v>207</v>
+      <c r="B54" s="6">
+        <v>195</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2250,67 +2339,67 @@
         <v>53</v>
       </c>
       <c r="B55" s="8">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>173</v>
+        <v>50</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A56" s="8">
         <v>54</v>
       </c>
       <c r="B56" s="8">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A57" s="8">
         <v>55</v>
       </c>
       <c r="B57" s="8">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>177</v>
+        <v>53</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A58" s="8">
         <v>56</v>
       </c>
       <c r="B58" s="8">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2318,33 +2407,33 @@
         <v>57</v>
       </c>
       <c r="B59" s="8">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D59" s="6" t="s">
-        <v>181</v>
+        <v>55</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>171</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="67.5" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A60" s="8">
         <v>58</v>
       </c>
       <c r="B60" s="8">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2352,84 +2441,84 @@
         <v>59</v>
       </c>
       <c r="B61" s="8">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>60</v>
+        <v>174</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A62" s="8">
         <v>60</v>
       </c>
       <c r="B62" s="8">
-        <v>247</v>
+        <v>217</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A63" s="8">
         <v>61</v>
       </c>
       <c r="B63" s="8">
-        <v>249</v>
+        <v>223</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>62</v>
+        <v>244</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A64" s="8">
         <v>62</v>
       </c>
       <c r="B64" s="8">
-        <v>263</v>
+        <v>234</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A65" s="8">
         <v>63</v>
       </c>
       <c r="B65" s="8">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2437,16 +2526,16 @@
         <v>64</v>
       </c>
       <c r="B66" s="8">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2454,16 +2543,16 @@
         <v>65</v>
       </c>
       <c r="B67" s="8">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>196</v>
+        <v>61</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>185</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2471,33 +2560,33 @@
         <v>66</v>
       </c>
       <c r="B68" s="8">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="54" x14ac:dyDescent="0.2">
       <c r="A69" s="8">
         <v>67</v>
       </c>
       <c r="B69" s="8">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>149</v>
+        <v>189</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2505,16 +2594,16 @@
         <v>68</v>
       </c>
       <c r="B70" s="8">
-        <v>320</v>
+        <v>271</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>201</v>
+        <v>64</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>190</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2522,16 +2611,16 @@
         <v>69</v>
       </c>
       <c r="B71" s="8">
-        <v>327</v>
+        <v>273</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>69</v>
+        <v>245</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>203</v>
+        <v>246</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>204</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2539,16 +2628,16 @@
         <v>70</v>
       </c>
       <c r="B72" s="8">
-        <v>330</v>
+        <v>276</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>205</v>
+        <v>192</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2556,67 +2645,67 @@
         <v>71</v>
       </c>
       <c r="B73" s="8">
-        <v>332</v>
+        <v>285</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>207</v>
+        <v>66</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>194</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A74" s="8">
         <v>72</v>
       </c>
       <c r="B74" s="8">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>73</v>
       </c>
       <c r="B75" s="8">
-        <v>342</v>
+        <v>293</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="27" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>74</v>
       </c>
       <c r="B76" s="8">
-        <v>349</v>
+        <v>320</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>213</v>
+        <v>230</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>199</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2624,16 +2713,16 @@
         <v>75</v>
       </c>
       <c r="B77" s="8">
-        <v>351</v>
+        <v>327</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2641,33 +2730,33 @@
         <v>76</v>
       </c>
       <c r="B78" s="8">
-        <v>356</v>
+        <v>330</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>77</v>
       </c>
       <c r="B79" s="8">
-        <v>359</v>
+        <v>332</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2675,69 +2764,195 @@
         <v>78</v>
       </c>
       <c r="B80" s="8">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>219</v>
+        <v>72</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>79</v>
       </c>
       <c r="B81" s="8">
+        <v>340</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+      <c r="A82" s="8">
+        <v>80</v>
+      </c>
+      <c r="B82" s="8">
+        <v>342</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E82" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A83" s="8">
+        <v>81</v>
+      </c>
+      <c r="B83" s="8">
+        <v>349</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A84" s="8">
+        <v>82</v>
+      </c>
+      <c r="B84" s="8">
+        <v>351</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
+      <c r="A85" s="8">
+        <v>83</v>
+      </c>
+      <c r="B85" s="8">
+        <v>352</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="54" x14ac:dyDescent="0.2">
+      <c r="A86" s="8">
+        <v>84</v>
+      </c>
+      <c r="B86" s="8">
+        <v>356</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="8">
+        <v>85</v>
+      </c>
+      <c r="B87" s="8">
+        <v>359</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+      <c r="A88" s="8">
+        <v>86</v>
+      </c>
+      <c r="B88" s="8">
+        <v>361</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E88" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="27" x14ac:dyDescent="0.2">
+      <c r="A89" s="8">
+        <v>87</v>
+      </c>
+      <c r="B89" s="8">
         <v>362</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C89" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D81" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-    </row>
-    <row r="83" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E83" s="2"/>
-    </row>
-    <row r="84" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E84" s="2"/>
-    </row>
-    <row r="85" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E85" s="2"/>
-    </row>
-    <row r="86" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E86" s="2"/>
-    </row>
-    <row r="87" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E87" s="2"/>
-    </row>
-    <row r="88" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E88" s="2"/>
-    </row>
-    <row r="89" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="E89" s="2"/>
+      <c r="D89" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E93" s="2"/>
+    </row>
+    <row r="94" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E94" s="2"/>
+    </row>
+    <row r="95" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E95" s="2"/>
+    </row>
+    <row r="96" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="E96" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A82:E82"/>
   </mergeCells>
   <pageMargins left="0.38" right="0.26" top="0.4" bottom="0.42" header="0.3" footer="0.3"/>
   <pageSetup scale="67" fitToHeight="4" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
feat (paper info): update name data
</commit_message>
<xml_diff>
--- a/data/accepted.xlsx
+++ b/data/accepted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GitHub\icmc-website\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DD23BD-4F8E-4ABD-81D4-699ADD3331C7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9CD652-3A6A-4A0C-8E8C-08E33BBC1286}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="4215" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -442,10 +442,6 @@
 Nadia El Mrabet
 Alexandre Berzati
 Jean-Baptiste Rigaud</t>
-  </si>
-  <si>
-    <t>Mohamed Fazil Mohamed Firdhous
-Rahmat Budiarto</t>
   </si>
   <si>
     <t>University of Moratuwa, Sri Lanka
@@ -1070,6 +1066,10 @@
   <si>
     <t>University of Fukui, Japan
 University of Fukui, Japan</t>
+  </si>
+  <si>
+    <t>M F M Firdhous
+Rahmat Budiarto</t>
   </si>
 </sst>
 </file>
@@ -1412,8 +1412,8 @@
   </sheetPr>
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1428,7 +1428,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -1596,13 +1596,13 @@
         <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1613,7 +1613,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>95</v>
@@ -1687,7 +1687,7 @@
         <v>104</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -1698,13 +1698,13 @@
         <v>68</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>221</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
@@ -1800,7 +1800,7 @@
         <v>93</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>111</v>
@@ -1817,13 +1817,13 @@
         <v>97</v>
       </c>
       <c r="C24" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>236</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1874,7 +1874,7 @@
         <v>118</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1888,10 +1888,10 @@
         <v>26</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -1905,10 +1905,10 @@
         <v>27</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1922,10 +1922,10 @@
         <v>28</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>123</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -1936,13 +1936,13 @@
         <v>116</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="E31" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
@@ -1959,7 +1959,7 @@
         <v>29</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1973,10 +1973,10 @@
         <v>31</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -1990,10 +1990,10 @@
         <v>32</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2010,7 +2010,7 @@
         <v>33</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2038,13 +2038,13 @@
         <v>127</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="5" t="s">
         <v>135</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2058,10 +2058,10 @@
         <v>36</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2075,7 +2075,7 @@
         <v>37</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>114</v>
@@ -2092,10 +2092,10 @@
         <v>38</v>
       </c>
       <c r="D40" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
@@ -2112,7 +2112,7 @@
         <v>39</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2126,10 +2126,10 @@
         <v>41</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>143</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2143,10 +2143,10 @@
         <v>42</v>
       </c>
       <c r="D43" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2160,10 +2160,10 @@
         <v>43</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>147</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="81" x14ac:dyDescent="0.2">
@@ -2177,10 +2177,10 @@
         <v>44</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2194,10 +2194,10 @@
         <v>45</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>150</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
@@ -2208,13 +2208,13 @@
         <v>156</v>
       </c>
       <c r="C47" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="E47" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2225,13 +2225,13 @@
         <v>157</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D48" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2245,10 +2245,10 @@
         <v>46</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2259,13 +2259,13 @@
         <v>164</v>
       </c>
       <c r="C50" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="E50" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2279,10 +2279,10 @@
         <v>47</v>
       </c>
       <c r="D51" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>156</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2296,10 +2296,10 @@
         <v>48</v>
       </c>
       <c r="D52" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2310,13 +2310,13 @@
         <v>191</v>
       </c>
       <c r="C53" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D53" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="E53" s="5" t="s">
         <v>161</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2330,10 +2330,10 @@
         <v>49</v>
       </c>
       <c r="D54" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>163</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2347,10 +2347,10 @@
         <v>50</v>
       </c>
       <c r="D55" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>252</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2364,10 +2364,10 @@
         <v>51</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2381,10 +2381,10 @@
         <v>52</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2398,10 +2398,10 @@
         <v>53</v>
       </c>
       <c r="D58" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>167</v>
-      </c>
-      <c r="E58" s="5" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2415,10 +2415,10 @@
         <v>54</v>
       </c>
       <c r="D59" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2432,10 +2432,10 @@
         <v>55</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2446,13 +2446,13 @@
         <v>216</v>
       </c>
       <c r="C61" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="E61" s="5" t="s">
         <v>173</v>
-      </c>
-      <c r="E61" s="5" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2466,10 +2466,10 @@
         <v>56</v>
       </c>
       <c r="D62" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>175</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="13.5" x14ac:dyDescent="0.2">
@@ -2480,13 +2480,13 @@
         <v>223</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D63" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2500,10 +2500,10 @@
         <v>57</v>
       </c>
       <c r="D64" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="67.5" x14ac:dyDescent="0.2">
@@ -2517,10 +2517,10 @@
         <v>58</v>
       </c>
       <c r="D65" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2534,10 +2534,10 @@
         <v>59</v>
       </c>
       <c r="D66" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>181</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2551,10 +2551,10 @@
         <v>60</v>
       </c>
       <c r="D67" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2568,10 +2568,10 @@
         <v>61</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2585,10 +2585,10 @@
         <v>62</v>
       </c>
       <c r="D69" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="E69" s="5" t="s">
         <v>186</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2602,10 +2602,10 @@
         <v>63</v>
       </c>
       <c r="D70" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E70" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2616,13 +2616,13 @@
         <v>273</v>
       </c>
       <c r="C71" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D71" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="E71" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="E71" s="5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2636,10 +2636,10 @@
         <v>64</v>
       </c>
       <c r="D72" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E72" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2653,10 +2653,10 @@
         <v>65</v>
       </c>
       <c r="D73" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E73" s="5" t="s">
         <v>192</v>
-      </c>
-      <c r="E73" s="5" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2670,10 +2670,10 @@
         <v>66</v>
       </c>
       <c r="D74" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="E74" s="5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2687,10 +2687,10 @@
         <v>67</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2701,13 +2701,13 @@
         <v>320</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D76" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E76" s="5" t="s">
         <v>197</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2721,10 +2721,10 @@
         <v>68</v>
       </c>
       <c r="D77" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="E77" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2738,10 +2738,10 @@
         <v>69</v>
       </c>
       <c r="D78" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E78" s="5" t="s">
         <v>201</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2755,10 +2755,10 @@
         <v>70</v>
       </c>
       <c r="D79" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E79" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2772,10 +2772,10 @@
         <v>71</v>
       </c>
       <c r="D80" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E80" s="5" t="s">
         <v>205</v>
-      </c>
-      <c r="E80" s="5" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="67.5" x14ac:dyDescent="0.2">
@@ -2789,10 +2789,10 @@
         <v>72</v>
       </c>
       <c r="D81" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E81" s="5" t="s">
         <v>246</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2806,10 +2806,10 @@
         <v>72</v>
       </c>
       <c r="D82" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E82" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="E82" s="5" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2823,10 +2823,10 @@
         <v>73</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2840,10 +2840,10 @@
         <v>74</v>
       </c>
       <c r="D84" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E84" s="5" t="s">
         <v>210</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="40.5" x14ac:dyDescent="0.2">
@@ -2854,13 +2854,13 @@
         <v>352</v>
       </c>
       <c r="C85" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D85" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="D85" s="6" t="s">
-        <v>249</v>
-      </c>
       <c r="E85" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="54" x14ac:dyDescent="0.2">
@@ -2874,10 +2874,10 @@
         <v>75</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2891,10 +2891,10 @@
         <v>76</v>
       </c>
       <c r="D87" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E87" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2905,13 +2905,13 @@
         <v>361</v>
       </c>
       <c r="C88" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D88" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="E88" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="E88" s="5" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="27" x14ac:dyDescent="0.2">
@@ -2925,10 +2925,10 @@
         <v>77</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>